<commit_message>
summary of simulation results
</commit_message>
<xml_diff>
--- a/SUMMARY/07-16-2014 - FP&SAV - Scheffer - highershading - lowerinitialcover - size and shape/simulation_summary_07-16-2014.xlsx
+++ b/SUMMARY/07-16-2014 - FP&SAV - Scheffer - highershading - lowerinitialcover - size and shape/simulation_summary_07-16-2014.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Functions used:</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>7/16/2014 11:52AM</t>
   </si>
 </sst>
 </file>
@@ -401,6 +404,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,9 +425,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -755,7 +758,9 @@
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
@@ -775,10 +780,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="21"/>
       <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
@@ -819,10 +824,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="20"/>
       <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
@@ -842,10 +847,10 @@
       <c r="B12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -908,7 +913,7 @@
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="17" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -935,11 +940,11 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
@@ -982,7 +987,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="4">
@@ -999,7 +1004,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="4">
@@ -1016,7 +1021,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B25" s="4">

</xml_diff>

<commit_message>
Re-organizing files & re-doing simulation inputs
</commit_message>
<xml_diff>
--- a/SUMMARY/07-16-2014 - FP&SAV - Scheffer - highershading - lowerinitialcover - size and shape/simulation_summary_07-16-2014.xlsx
+++ b/SUMMARY/07-16-2014 - FP&SAV - Scheffer - highershading - lowerinitialcover - size and shape/simulation_summary_07-16-2014.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Functions used:</t>
   </si>
@@ -217,58 +217,55 @@
     <t>amnt_colonize_FP</t>
   </si>
   <si>
-    <t>input23.csv</t>
-  </si>
-  <si>
-    <t>output23.csv</t>
-  </si>
-  <si>
     <t>Functions not used</t>
   </si>
   <si>
+    <t>initial_perc_SAV_cover</t>
+  </si>
+  <si>
+    <t>initial_perc_FP_cover</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>lightlimitationSAV</t>
+  </si>
+  <si>
+    <t>lightlimitation01</t>
+  </si>
+  <si>
+    <t>shadingbyFP</t>
+  </si>
+  <si>
+    <t>4, 0.2</t>
+  </si>
+  <si>
+    <t>input24.csv</t>
+  </si>
+  <si>
+    <t>output24.csv</t>
+  </si>
+  <si>
+    <t>SUMMARIZE12.R</t>
+  </si>
+  <si>
+    <t>7/16/2014 ~9:30AM</t>
+  </si>
+  <si>
+    <t>replicates</t>
+  </si>
+  <si>
+    <t>1,15,30,60</t>
+  </si>
+  <si>
     <t>07-16-2014 - FP&amp;SAV - Scheffer - highershading - lowerinitialcover</t>
   </si>
   <si>
-    <t>initial_perc_SAV_cover</t>
-  </si>
-  <si>
-    <t>initial_perc_FP_cover</t>
-  </si>
-  <si>
-    <t>1, 15, 30, 60</t>
-  </si>
-  <si>
     <t>wind_shape2</t>
-  </si>
-  <si>
-    <t>SUMMARIZE12.R</t>
-  </si>
-  <si>
-    <t>7/16/2014 ~9:30AM</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>lightlimitationSAV</t>
-  </si>
-  <si>
-    <t>lightlimitation01</t>
-  </si>
-  <si>
-    <t>shadingbyFP</t>
-  </si>
-  <si>
-    <t>replicates</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>7/16/2014 11:52AM</t>
   </si>
 </sst>
 </file>
@@ -383,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -404,9 +401,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,7 +725,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -748,7 +744,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>17</v>
@@ -758,9 +754,7 @@
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
@@ -780,10 +774,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="20"/>
       <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
@@ -804,7 +798,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -812,10 +806,10 @@
         <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,10 +818,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="19"/>
       <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
@@ -847,10 +841,10 @@
       <c r="B12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -875,7 +869,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F14" s="6">
         <v>40</v>
@@ -889,7 +883,7 @@
         <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F15" s="6">
         <v>40</v>
@@ -913,8 +907,8 @@
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>75</v>
+      <c r="B17" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>6</v>
@@ -940,11 +934,11 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
@@ -987,14 +981,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>71</v>
+      <c r="A23" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="4">
         <v>4</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>16</v>
@@ -1004,14 +998,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>72</v>
+      <c r="A24" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="B24" s="4">
         <v>4</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>20</v>
@@ -1021,14 +1015,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>82</v>
+      <c r="A25" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>21</v>
@@ -1073,12 +1067,12 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="E29" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F29" s="4">
         <v>0.01</v>
@@ -1086,7 +1080,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E30" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F30" s="4">
         <v>0.01</v>
@@ -1094,7 +1088,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F31" s="4">
         <v>0.04</v>
@@ -1110,7 +1104,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E33" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F33" s="4">
         <v>0.4</v>

</xml_diff>